<commit_message>
finished SORT feature + scrum sheet
</commit_message>
<xml_diff>
--- a/P11/store/Scrum.xlsx
+++ b/P11/store/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P11/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2675EC4E-40F0-8448-B758-E9940B159F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAFCB6D-7619-D64D-A0DB-2172E11C232A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="212">
   <si>
     <t>Product Name:</t>
   </si>
@@ -672,6 +672,12 @@
   </si>
   <si>
     <t>Finished in Sprint 5</t>
+  </si>
+  <si>
+    <t>Write and implement method compareTo for Customer.java</t>
+  </si>
+  <si>
+    <t>change Store.customers field from HashSet to TreeSet</t>
   </si>
 </sst>
 </file>
@@ -2750,13 +2756,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3870,8 +3876,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5019,7 +5025,9 @@
       <c r="F46" s="17">
         <v>5</v>
       </c>
-      <c r="G46" s="17"/>
+      <c r="G46" s="17" t="s">
+        <v>209</v>
+      </c>
       <c r="H46" s="18" t="s">
         <v>31</v>
       </c>
@@ -10805,7 +10813,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10910,7 +10918,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -10925,7 +10933,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -10943,7 +10951,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -10965,7 +10973,7 @@
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -11123,34 +11131,52 @@
       </c>
       <c r="F19" s="38"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="35" t="s">
+        <v>109</v>
+      </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="37"/>
+      <c r="D20" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>208</v>
+      </c>
       <c r="F20" s="38"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="35" t="s">
+        <v>109</v>
+      </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="37"/>
+      <c r="D21" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>208</v>
+      </c>
       <c r="F21" s="38"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="35" t="s">
+        <v>109</v>
+      </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="37"/>
+      <c r="D22" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>208</v>
+      </c>
       <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
finish GSAVE feature + interface Saveable + finished scrum sheet
</commit_message>
<xml_diff>
--- a/P11/store/Scrum.xlsx
+++ b/P11/store/Scrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P11/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AAFCB6D-7619-D64D-A0DB-2172E11C232A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EAD982-4697-F24D-AEF7-693C4A1E805F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="215">
   <si>
     <t>Product Name:</t>
   </si>
@@ -678,6 +678,15 @@
   </si>
   <si>
     <t>change Store.customers field from HashSet to TreeSet</t>
+  </si>
+  <si>
+    <t>Implement the interface Saveable with its abstract method</t>
+  </si>
+  <si>
+    <t>Update other related files to implement Saveable</t>
+  </si>
+  <si>
+    <t>Write the private generic save method in Store.java + necessary calls</t>
   </si>
 </sst>
 </file>
@@ -2756,13 +2765,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3876,8 +3885,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5058,7 +5067,9 @@
       <c r="F47" s="17">
         <v>5</v>
       </c>
-      <c r="G47" s="17"/>
+      <c r="G47" s="17" t="s">
+        <v>209</v>
+      </c>
       <c r="H47" s="18" t="s">
         <v>70</v>
       </c>
@@ -10812,8 +10823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10918,7 +10929,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -10933,7 +10944,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -10951,7 +10962,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -10973,7 +10984,7 @@
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -11179,34 +11190,52 @@
       </c>
       <c r="F22" s="38"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="35" t="s">
+        <v>113</v>
+      </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="37"/>
+      <c r="D23" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>208</v>
+      </c>
       <c r="F23" s="38"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="35" t="s">
+        <v>113</v>
+      </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="37"/>
+      <c r="D24" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>208</v>
+      </c>
       <c r="F24" s="38"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="35" t="s">
+        <v>113</v>
+      </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37"/>
+      <c r="D25" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>208</v>
+      </c>
       <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>